<commit_message>
BARD1 Filtering bug fixes
BARD1 filtering bug fixed with start and end coordinates in input file swapped
</commit_message>
<xml_diff>
--- a/Data/SNV_filtering_inputs/20250415_BARD1_filter_entry.xlsx
+++ b/Data/SNV_filtering_inputs/20250415_BARD1_filter_entry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Documents/GitHub/BARD1_SGE_analysis/Data/SNV_filtering_inputs/PillarProject_filtering/BARD1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Documents/GitHub/BARD1_SGE_analysis/Data/SNV_filtering_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3355832-8B67-C644-BB2C-D0517CE2B78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81297937-E565-7C48-9F19-7AF65379060D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="620" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="targets" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B100B6-3216-FE4F-97CE-2991D8618EC1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1037,10 +1037,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>214725646</v>
+      </c>
+      <c r="B2">
         <v>214809683</v>
-      </c>
-      <c r="B2">
-        <v>214725646</v>
       </c>
       <c r="C2">
         <v>0</v>

</xml_diff>